<commit_message>
work and 1 def
</commit_message>
<xml_diff>
--- a/aldo_1c.xlsx
+++ b/aldo_1c.xlsx
@@ -413,51 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>298044</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>8</v>
-      </c>
-      <c r="D1" t="n">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>298044</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>161</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
work while xlsx file
</commit_message>
<xml_diff>
--- a/aldo_1c.xlsx
+++ b/aldo_1c.xlsx
@@ -413,14 +413,123 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>298044</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D1" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>298044</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>298044</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>298044</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>298044</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>298044</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Диск DVD+R 10шт Mirex 4.7Gb 16x Cake box printable inkjet (UL130029A1L)</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>